<commit_message>
PRJ0019297 CVAS Time Tracking Changes+ changes after SB Referesh
</commit_message>
<xml_diff>
--- a/TestData/TMTI0055011_VerifyInternalDealTeamSpecialtyRoleIncreasedLimitForFVALOBOpportunityEngagement.xlsx
+++ b/TestData/TMTI0055011_VerifyInternalDealTeamSpecialtyRoleIncreasedLimitForFVALOBOpportunityEngagement.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vijay.kumar\source\repos\SalesForce_Project\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VKumar0427\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE905AFB-15E3-4CBD-8D3A-AD425754B11A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB8CCB78-CDEE-4E85-AF5F-488A17920D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="5" xr2:uid="{4F41EB50-8C78-4F9F-A1D4-8B783E020697}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14640" firstSheet="1" activeTab="3" xr2:uid="{4F41EB50-8C78-4F9F-A1D4-8B783E020697}"/>
   </bookViews>
   <sheets>
     <sheet name="AddOpportunity" sheetId="1" r:id="rId1"/>
@@ -259,9 +259,6 @@
     <t>Dimitri Drone</t>
   </si>
   <si>
-    <t>Jason Vierig</t>
-  </si>
-  <si>
     <t>Karim Jooma</t>
   </si>
   <si>
@@ -338,6 +335,9 @@
   </si>
   <si>
     <t>OppDealTeamMembers</t>
+  </si>
+  <si>
+    <t>Mark Schade</t>
   </si>
 </sst>
 </file>
@@ -730,9 +730,9 @@
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -821,7 +821,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -923,9 +923,9 @@
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>50</v>
       </c>
@@ -933,7 +933,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -954,9 +954,9 @@
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>53</v>
       </c>
@@ -982,7 +982,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -1017,153 +1017,153 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53E8CB76-FB8A-4028-8972-B88CE86EF1D8}">
   <dimension ref="A1:A28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
-        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1179,19 +1179,19 @@
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1203,30 +1203,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41831907-90E4-4F72-A4FC-60E82CC27F92}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="76.21875" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" customWidth="1"/>
+    <col min="1" max="1" width="76.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>96</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>